<commit_message>
aadhaar name typos fixed . Aadhaar made mandatory and unique
Null fields are fixed . Any field if null is now empty.
</commit_message>
<xml_diff>
--- a/source/A_CERTIFICATES.xlsx
+++ b/source/A_CERTIFICATES.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="7" r:id="rId1"/>
@@ -200,7 +200,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,13 +262,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF002060"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -290,7 +283,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -313,6 +306,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -335,62 +413,80 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -714,251 +810,260 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA11"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="7" t="s">
+      <c r="K1" s="17"/>
+      <c r="L1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="4" t="s">
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="19"/>
     </row>
-    <row r="2" spans="1:27" ht="72" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="10" t="s">
+    <row r="2" spans="1:26" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10" t="s">
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="11" t="s">
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="S2" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="12" t="s">
+      <c r="T2" s="22"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="4" t="s">
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="51" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="13" t="s">
+    <row r="3" spans="1:26" ht="51" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="L3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="M3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="N3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="O3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="P3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="Q3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="R3" s="16" t="s">
+      <c r="R3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="14" t="s">
+      <c r="S3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="T3" s="14" t="s">
+      <c r="T3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="U3" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="17" t="s">
+      <c r="V3" s="22"/>
+      <c r="W3" s="22"/>
+      <c r="X3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="Y3" s="17" t="s">
+      <c r="Y3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Z3" s="4"/>
+      <c r="Z3" s="22"/>
     </row>
-    <row r="4" spans="1:27" s="1" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:26" s="1" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="K4" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="18" t="s">
+      <c r="L4" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="M4" s="18" t="s">
+      <c r="M4" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="N4" s="18" t="s">
+      <c r="N4" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="O4" s="18" t="s">
+      <c r="O4" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="P4" s="18" t="s">
+      <c r="P4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="Q4" s="18" t="s">
+      <c r="Q4" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="R4" s="18" t="s">
+      <c r="R4" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="S4" s="18" t="s">
+      <c r="S4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="T4" s="18" t="s">
+      <c r="T4" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="U4" s="18" t="s">
+      <c r="U4" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="V4" s="18" t="s">
+      <c r="V4" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="W4" s="18" t="s">
+      <c r="W4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="X4" s="18" t="s">
+      <c r="X4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="Y4" s="18" t="s">
+      <c r="Y4" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="Z4" s="18" t="s">
+      <c r="Z4" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="AA4" s="2"/>
     </row>
-    <row r="5" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:26" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I1:I3"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
     <mergeCell ref="Z2:Z3"/>
     <mergeCell ref="J1:K2"/>
     <mergeCell ref="L1:U1"/>
@@ -968,16 +1073,6 @@
     <mergeCell ref="O2:Q2"/>
     <mergeCell ref="S2:U2"/>
     <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I1:I3"/>
-    <mergeCell ref="L2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Camp list add or remove works fine
</commit_message>
<xml_diff>
--- a/source/A_CERTIFICATES.xlsx
+++ b/source/A_CERTIFICATES.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Date of Birth</t>
   </si>
@@ -194,6 +194,12 @@
   </si>
   <si>
     <t>Student Name</t>
+  </si>
+  <si>
+    <t>Institution</t>
+  </si>
+  <si>
+    <t>(ab)</t>
   </si>
 </sst>
 </file>
@@ -283,7 +289,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -319,6 +325,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -341,22 +371,37 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -369,31 +414,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -717,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,260 +767,269 @@
     <col min="1" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:27" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="9" t="s">
+      <c r="K1" s="13"/>
+      <c r="L1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="5" t="s">
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="W1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="X1" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
     </row>
-    <row r="2" spans="1:26" s="1" customFormat="1" ht="27.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="11" t="s">
+    <row r="2" spans="1:27" s="1" customFormat="1" ht="27.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="11" t="s">
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="12" t="s">
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="S2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="13" t="s">
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="5" t="s">
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="1" customFormat="1" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="14" t="s">
+    <row r="3" spans="1:27" s="1" customFormat="1" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="M3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="N3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="O3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="P3" s="15" t="s">
+      <c r="P3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Q3" s="17" t="s">
+      <c r="Q3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="R3" s="17" t="s">
+      <c r="R3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="15" t="s">
+      <c r="S3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="T3" s="15" t="s">
+      <c r="T3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="U3" s="17" t="s">
+      <c r="U3" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="18" t="s">
+      <c r="V3" s="13"/>
+      <c r="W3" s="13"/>
+      <c r="X3" s="23"/>
+      <c r="Y3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="Y3" s="18" t="s">
+      <c r="Z3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="Z3" s="8"/>
+      <c r="AA3" s="13"/>
     </row>
-    <row r="4" spans="1:26" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+    <row r="4" spans="1:27" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="M4" s="19" t="s">
+      <c r="M4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="N4" s="19" t="s">
+      <c r="N4" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="O4" s="19" t="s">
+      <c r="O4" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="P4" s="19" t="s">
+      <c r="P4" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="Q4" s="19" t="s">
+      <c r="Q4" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="R4" s="19" t="s">
+      <c r="R4" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="S4" s="19" t="s">
+      <c r="S4" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="T4" s="19" t="s">
+      <c r="T4" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="U4" s="19" t="s">
+      <c r="U4" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="V4" s="19" t="s">
+      <c r="V4" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="W4" s="19" t="s">
+      <c r="W4" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="X4" s="19" t="s">
+      <c r="X4" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="Y4" s="19" t="s">
+      <c r="Y4" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="Z4" s="19" t="s">
+      <c r="Z4" s="10" t="s">
         <v>56</v>
       </c>
+      <c r="AA4" s="10" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="J1:K2"/>
-    <mergeCell ref="L1:U1"/>
-    <mergeCell ref="W1:W3"/>
-    <mergeCell ref="X1:Z1"/>
-    <mergeCell ref="V1:V3"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="X2:Y2"/>
+  <mergeCells count="20">
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I1:I3"/>
+    <mergeCell ref="L2:N2"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I1:I3"/>
-    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="J1:K2"/>
+    <mergeCell ref="L1:U1"/>
+    <mergeCell ref="W1:W3"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="V1:V3"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="X1:X3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
intermediate aadhaar based excel to database
</commit_message>
<xml_diff>
--- a/source/A_CERTIFICATES.xlsx
+++ b/source/A_CERTIFICATES.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="A" sheetId="7" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -190,9 +190,6 @@
     <t>Grand Total  500</t>
   </si>
   <si>
-    <t>Ebrolment Number</t>
-  </si>
-  <si>
     <t>Student Name</t>
   </si>
   <si>
@@ -200,6 +197,9 @@
   </si>
   <si>
     <t>(ab)</t>
+  </si>
+  <si>
+    <t>Enrolment Number</t>
   </si>
 </sst>
 </file>
@@ -404,26 +404,26 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -512,7 +512,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -547,7 +547,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -758,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="AA4" sqref="AA4"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,17 +768,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>58</v>
+      <c r="A1" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>59</v>
+      <c r="D1" s="16" t="s">
+        <v>58</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>2</v>
@@ -799,7 +799,7 @@
         <v>6</v>
       </c>
       <c r="K1" s="13"/>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="18" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="13"/>
@@ -818,9 +818,9 @@
         <v>8</v>
       </c>
       <c r="X1" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y1" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y1" s="19" t="s">
         <v>9</v>
       </c>
       <c r="Z1" s="13"/>
@@ -838,12 +838,12 @@
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
       <c r="K2" s="13"/>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="14" t="s">
         <v>11</v>
       </c>
       <c r="M2" s="13"/>
       <c r="N2" s="13"/>
-      <c r="O2" s="16" t="s">
+      <c r="O2" s="14" t="s">
         <v>12</v>
       </c>
       <c r="P2" s="13"/>
@@ -859,7 +859,7 @@
       <c r="V2" s="13"/>
       <c r="W2" s="13"/>
       <c r="X2" s="22"/>
-      <c r="Y2" s="18" t="s">
+      <c r="Y2" s="20" t="s">
         <v>15</v>
       </c>
       <c r="Z2" s="13"/>
@@ -1004,22 +1004,12 @@
         <v>56</v>
       </c>
       <c r="AA4" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I1:I3"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
     <mergeCell ref="AA2:AA3"/>
     <mergeCell ref="J1:K2"/>
     <mergeCell ref="L1:U1"/>
@@ -1030,6 +1020,16 @@
     <mergeCell ref="S2:U2"/>
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="X1:X3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I1:I3"/>
+    <mergeCell ref="L2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
[stable ] backup before merging
</commit_message>
<xml_diff>
--- a/source/A_CERTIFICATES.xlsx
+++ b/source/A_CERTIFICATES.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="A" sheetId="7" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -199,7 +199,7 @@
     <t>(ab)</t>
   </si>
   <si>
-    <t>Enrolment Number</t>
+    <t>Enolment Number</t>
   </si>
 </sst>
 </file>
@@ -512,7 +512,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -547,7 +547,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -759,7 +759,7 @@
   <dimension ref="A1:AA11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>